<commit_message>
Final updates for February 2023 statistics
</commit_message>
<xml_diff>
--- a/statistics_files/2023/2023.z.graph.xlsx
+++ b/statistics_files/2023/2023.z.graph.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20394"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20395"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\George\Documents\github\next_statistics\statistics_files\2023\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\George\Documents\GitHub\next_statistics\statistics_files\2023\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F1133F9-32F8-4F77-9CCD-35478674583D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B449FBF-E5C8-4446-9F6F-06E3653110D5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11690" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11685" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1046,6 +1046,9 @@
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>89666</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>84022</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2131,15 +2134,15 @@
   <dimension ref="A1:F30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.7265625" customWidth="1"/>
+    <col min="1" max="1" width="15.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2159,7 +2162,7 @@
         <v>2023</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -2179,7 +2182,7 @@
         <v>89666</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -2195,8 +2198,11 @@
       <c r="E3">
         <v>74752</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F3">
+        <v>84022</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -2213,7 +2219,7 @@
         <v>90284</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -2230,7 +2236,7 @@
         <v>82578</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -2247,7 +2253,7 @@
         <v>90284</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -2264,7 +2270,7 @@
         <v>115115</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -2281,7 +2287,7 @@
         <v>102360</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -2298,7 +2304,7 @@
         <v>101787</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -2315,7 +2321,7 @@
         <v>90267</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -2332,7 +2338,7 @@
         <v>87376</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -2349,7 +2355,7 @@
         <v>84228</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -2366,7 +2372,7 @@
         <v>76918</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>13</v>
       </c>
@@ -2376,7 +2382,7 @@
       <c r="E16" s="3"/>
       <c r="F16" s="1"/>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="3"/>
       <c r="B17" s="3"/>
       <c r="C17" s="3"/>
@@ -2384,7 +2390,7 @@
       <c r="E17" s="3"/>
       <c r="F17" s="1"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="3"/>
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
@@ -2392,7 +2398,7 @@
       <c r="E18" s="3"/>
       <c r="F18" s="1"/>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="3"/>
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
@@ -2400,7 +2406,7 @@
       <c r="E19" s="3"/>
       <c r="F19" s="1"/>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="3"/>
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
@@ -2408,7 +2414,7 @@
       <c r="E20" s="3"/>
       <c r="F20" s="1"/>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="3"/>
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
@@ -2416,7 +2422,7 @@
       <c r="E21" s="3"/>
       <c r="F21" s="1"/>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="3"/>
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
@@ -2424,7 +2430,7 @@
       <c r="E22" s="3"/>
       <c r="F22" s="1"/>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="3"/>
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>
@@ -2432,7 +2438,7 @@
       <c r="E23" s="3"/>
       <c r="F23" s="1"/>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="3"/>
       <c r="B24" s="3"/>
       <c r="C24" s="3"/>
@@ -2440,7 +2446,7 @@
       <c r="E24" s="3"/>
       <c r="F24" s="1"/>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="3"/>
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
@@ -2448,7 +2454,7 @@
       <c r="E25" s="3"/>
       <c r="F25" s="1"/>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="3"/>
       <c r="B26" s="3"/>
       <c r="C26" s="3"/>
@@ -2456,7 +2462,7 @@
       <c r="E26" s="3"/>
       <c r="F26" s="1"/>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="3"/>
       <c r="B27" s="3"/>
       <c r="C27" s="3"/>
@@ -2464,7 +2470,7 @@
       <c r="E27" s="3"/>
       <c r="F27" s="1"/>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="3"/>
       <c r="B28" s="3"/>
       <c r="C28" s="3"/>
@@ -2472,7 +2478,7 @@
       <c r="E28" s="3"/>
       <c r="F28" s="1"/>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="3"/>
       <c r="B29" s="3"/>
       <c r="C29" s="3"/>
@@ -2480,7 +2486,7 @@
       <c r="E29" s="3"/>
       <c r="F29" s="1"/>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="3"/>
       <c r="B30" s="3"/>
       <c r="C30" s="3"/>

</xml_diff>

<commit_message>
Add files from May and begin updates to main files
</commit_message>
<xml_diff>
--- a/statistics_files/2023/2023.z.graph.xlsx
+++ b/statistics_files/2023/2023.z.graph.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20396"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20398"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\George\Documents\GitHub\next_statistics\statistics_files\2023\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F99D910-F3CA-4FD7-9FF0-88D3EF7BA969}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93B89B57-B21F-4A86-AA5E-20B083890716}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11685" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1052,6 +1052,12 @@
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>98440</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>84778</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>95894</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2137,7 +2143,7 @@
   <dimension ref="A1:F30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2241,6 +2247,9 @@
       <c r="E5">
         <v>82578</v>
       </c>
+      <c r="F5">
+        <v>84778</v>
+      </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
@@ -2257,6 +2266,9 @@
       </c>
       <c r="E6">
         <v>90284</v>
+      </c>
+      <c r="F6">
+        <v>95894</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Fix problems with graph and graph generator spreadsheet
</commit_message>
<xml_diff>
--- a/statistics_files/2023/2023.z.graph.xlsx
+++ b/statistics_files/2023/2023.z.graph.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\George\Documents\GitHub\next_statistics\statistics_files\2023\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70020A86-6D46-4FCA-B1D6-9AD6F3592570}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C529C140-5136-46BA-B904-BCC1F3BC9C53}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11685" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1060,6 +1060,9 @@
                   <c:v>95894</c:v>
                 </c:pt>
                 <c:pt idx="5">
+                  <c:v>114493</c:v>
+                </c:pt>
+                <c:pt idx="6">
                   <c:v>101818</c:v>
                 </c:pt>
               </c:numCache>
@@ -2291,7 +2294,7 @@
         <v>115115</v>
       </c>
       <c r="F7">
-        <v>101818</v>
+        <v>114493</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -2309,6 +2312,9 @@
       </c>
       <c r="E8">
         <v>102360</v>
+      </c>
+      <c r="F8">
+        <v>101818</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Update individual files for December + a couple of others
</commit_message>
<xml_diff>
--- a/statistics_files/2023/2023.z.graph.xlsx
+++ b/statistics_files/2023/2023.z.graph.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20404"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20405"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\George\Documents\GitHub\next_statistics\statistics_files\2023\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF84FB55-6110-4024-9756-54962B3C5037}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0B24132-BEB8-4A68-A23A-20D39B55BD07}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11685" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1076,6 +1076,9 @@
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>84962</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>75603</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2425,6 +2428,9 @@
       <c r="E13">
         <v>76918</v>
       </c>
+      <c r="F13">
+        <v>75603</v>
+      </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">

</xml_diff>